<commit_message>
add Medic@ column for Curacion form in base export
</commit_message>
<xml_diff>
--- a/app/data/base_export.xlsx
+++ b/app/data/base_export.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhB1mJcL+w2UZ5mIBL9t9LCahdE0Q=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mj7mT2Kz5T2SbrjYfhO5eeRTnBiLw=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="485">
   <si>
     <t>Fecha de la visita</t>
   </si>
@@ -1459,6 +1459,9 @@
   </si>
   <si>
     <t>Cita de seguimiento</t>
+  </si>
+  <si>
+    <t>Medic@</t>
   </si>
   <si>
     <t>Infusión</t>
@@ -1522,7 +1525,6 @@
     <font>
       <b/>
       <color rgb="FF222222"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="12.0"/>
@@ -1905,7 +1907,7 @@
     <col customWidth="1" min="489" max="490" width="10.56"/>
     <col customWidth="1" min="491" max="491" width="12.44"/>
     <col customWidth="1" min="492" max="492" width="11.56"/>
-    <col customWidth="1" min="493" max="497" width="10.56"/>
+    <col customWidth="1" min="493" max="498" width="10.56"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -2499,9 +2501,9 @@
       <c r="RZ1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="SA1" s="7"/>
       <c r="SB1" s="7"/>
       <c r="SC1" s="7"/>
+      <c r="SD1" s="7"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="8"/>
@@ -3931,17 +3933,20 @@
       <c r="RY2" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="RZ2" s="11" t="s">
+      <c r="RZ2" s="13" t="s">
+        <v>481</v>
+      </c>
+      <c r="SA2" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="SA2" s="11" t="s">
-        <v>481</v>
       </c>
       <c r="SB2" s="11" t="s">
         <v>482</v>
       </c>
       <c r="SC2" s="11" t="s">
         <v>483</v>
+      </c>
+      <c r="SD2" s="11" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
@@ -4441,6 +4446,7 @@
       <c r="SA3" s="20"/>
       <c r="SB3" s="20"/>
       <c r="SC3" s="20"/>
+      <c r="SD3" s="20"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="17"/>
@@ -4939,6 +4945,7 @@
       <c r="SA4" s="20"/>
       <c r="SB4" s="20"/>
       <c r="SC4" s="20"/>
+      <c r="SD4" s="20"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="17"/>
@@ -5437,6 +5444,7 @@
       <c r="SA5" s="20"/>
       <c r="SB5" s="20"/>
       <c r="SC5" s="20"/>
+      <c r="SD5" s="20"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="17"/>
@@ -5508,6 +5516,7 @@
       <c r="SA6" s="20"/>
       <c r="SB6" s="20"/>
       <c r="SC6" s="20"/>
+      <c r="SD6" s="20"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="17"/>
@@ -5580,6 +5589,7 @@
       <c r="SA7" s="20"/>
       <c r="SB7" s="20"/>
       <c r="SC7" s="20"/>
+      <c r="SD7" s="20"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="17"/>
@@ -5650,6 +5660,7 @@
       <c r="SA8" s="20"/>
       <c r="SB8" s="20"/>
       <c r="SC8" s="20"/>
+      <c r="SD8" s="20"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="17"/>
@@ -5720,6 +5731,7 @@
       <c r="SA9" s="20"/>
       <c r="SB9" s="20"/>
       <c r="SC9" s="20"/>
+      <c r="SD9" s="20"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="17"/>
@@ -5792,6 +5804,7 @@
       <c r="SA10" s="20"/>
       <c r="SB10" s="20"/>
       <c r="SC10" s="20"/>
+      <c r="SD10" s="20"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="24"/>
@@ -5864,6 +5877,7 @@
       <c r="SA11" s="20"/>
       <c r="SB11" s="20"/>
       <c r="SC11" s="20"/>
+      <c r="SD11" s="20"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="24"/>
@@ -5933,6 +5947,7 @@
       <c r="SA12" s="20"/>
       <c r="SB12" s="20"/>
       <c r="SC12" s="20"/>
+      <c r="SD12" s="20"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="24"/>
@@ -6000,6 +6015,7 @@
       <c r="SA13" s="20"/>
       <c r="SB13" s="20"/>
       <c r="SC13" s="20"/>
+      <c r="SD13" s="20"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="20"/>
@@ -6064,6 +6080,7 @@
       <c r="SA14" s="20"/>
       <c r="SB14" s="20"/>
       <c r="SC14" s="20"/>
+      <c r="SD14" s="20"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="20"/>
@@ -6126,6 +6143,7 @@
       <c r="SA15" s="20"/>
       <c r="SB15" s="20"/>
       <c r="SC15" s="20"/>
+      <c r="SD15" s="20"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="20"/>
@@ -6186,6 +6204,7 @@
       <c r="SA16" s="20"/>
       <c r="SB16" s="20"/>
       <c r="SC16" s="20"/>
+      <c r="SD16" s="20"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="20"/>
@@ -6243,6 +6262,7 @@
       <c r="SA17" s="20"/>
       <c r="SB17" s="20"/>
       <c r="SC17" s="20"/>
+      <c r="SD17" s="20"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="20"/>
@@ -6298,6 +6318,7 @@
       <c r="SA18" s="20"/>
       <c r="SB18" s="20"/>
       <c r="SC18" s="20"/>
+      <c r="SD18" s="20"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="20"/>
@@ -6353,6 +6374,7 @@
       <c r="SA19" s="20"/>
       <c r="SB19" s="20"/>
       <c r="SC19" s="20"/>
+      <c r="SD19" s="20"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="20"/>
@@ -6405,6 +6427,7 @@
       <c r="SA20" s="20"/>
       <c r="SB20" s="20"/>
       <c r="SC20" s="20"/>
+      <c r="SD20" s="20"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="20"/>

</xml_diff>